<commit_message>
Tyler told me to commit
</commit_message>
<xml_diff>
--- a/Results/AIdrift_ai2_1 70h_W38334x0012ak1432180_75.xlsx
+++ b/Results/AIdrift_ai2_1 70h_W38334x0012ak1432180_75.xlsx
@@ -412,16 +412,16 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>0.1538461595773697</v>
       </c>
       <c r="D2" t="n">
-        <v>740</v>
+        <v>731</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -432,13 +432,13 @@
         <v>8.5</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.1538461595773697</v>
       </c>
       <c r="D3" t="n">
-        <v>740</v>
+        <v>731</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -449,13 +449,13 @@
         <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.1923076957464218</v>
       </c>
       <c r="D4" t="n">
-        <v>740</v>
+        <v>732</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -466,13 +466,13 @@
         <v>9.5</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.2307692319154739</v>
       </c>
       <c r="D5" t="n">
-        <v>740</v>
+        <v>733</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -483,13 +483,13 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.2307692319154739</v>
       </c>
       <c r="D6" t="n">
-        <v>740</v>
+        <v>733</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -500,13 +500,13 @@
         <v>10.5</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>0.2692307829856873</v>
       </c>
       <c r="D7" t="n">
-        <v>740</v>
+        <v>734</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -517,13 +517,13 @@
         <v>11</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>0.2692307829856873</v>
       </c>
       <c r="D8" t="n">
-        <v>740</v>
+        <v>734</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -534,13 +534,13 @@
         <v>11.5</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>0.2692307829856873</v>
       </c>
       <c r="D9" t="n">
-        <v>740</v>
+        <v>734</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -551,13 +551,13 @@
         <v>12</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>0.3076923191547394</v>
       </c>
       <c r="D10" t="n">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -568,13 +568,13 @@
         <v>12.5</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.1549186706542969</v>
+        <v>0.3076923191547394</v>
       </c>
       <c r="D11" t="n">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -585,13 +585,13 @@
         <v>13</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.03872966766357422</v>
+        <v>0.3076923191547394</v>
       </c>
       <c r="D12" t="n">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="E12" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -602,13 +602,13 @@
         <v>13.5</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>0.3076923191547394</v>
       </c>
       <c r="D13" t="n">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="E13" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -619,13 +619,13 @@
         <v>14</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.03872966766357422</v>
+        <v>0.3076923191547394</v>
       </c>
       <c r="D14" t="n">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="E14" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -636,13 +636,13 @@
         <v>14.5</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.03872966766357422</v>
+        <v>0.3076923191547394</v>
       </c>
       <c r="D15" t="n">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="E15" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -653,13 +653,13 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.03872966766357422</v>
+        <v>0.3076923191547394</v>
       </c>
       <c r="D16" t="n">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="E16" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -670,13 +670,13 @@
         <v>15.5</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.03872966766357422</v>
+        <v>0.3076923191547394</v>
       </c>
       <c r="D17" t="n">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="E17" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -687,13 +687,13 @@
         <v>16</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.07745933532714844</v>
+        <v>0.3076923191547394</v>
       </c>
       <c r="D18" t="n">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="E18" t="n">
-        <v>-2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -724,16 +724,16 @@
         <v>8</v>
       </c>
       <c r="C21" t="n">
-        <v>50</v>
+        <v>50.11538314819336</v>
       </c>
       <c r="D21" t="n">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
-        <v>2031</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -744,13 +744,13 @@
         <v>8.5</v>
       </c>
       <c r="C22" t="n">
-        <v>50.03860855102539</v>
+        <v>50.15384674072266</v>
       </c>
       <c r="D22" t="n">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -761,13 +761,13 @@
         <v>9</v>
       </c>
       <c r="C23" t="n">
-        <v>50.03860855102539</v>
+        <v>50.15384674072266</v>
       </c>
       <c r="D23" t="n">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -778,13 +778,13 @@
         <v>9.5</v>
       </c>
       <c r="C24" t="n">
-        <v>50</v>
+        <v>50.15384674072266</v>
       </c>
       <c r="D24" t="n">
         <v>2031</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -795,13 +795,13 @@
         <v>10</v>
       </c>
       <c r="C25" t="n">
-        <v>50</v>
+        <v>50.15384674072266</v>
       </c>
       <c r="D25" t="n">
         <v>2031</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -812,13 +812,13 @@
         <v>10.5</v>
       </c>
       <c r="C26" t="n">
-        <v>50.03860855102539</v>
+        <v>50.15384674072266</v>
       </c>
       <c r="D26" t="n">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -829,13 +829,13 @@
         <v>11</v>
       </c>
       <c r="C27" t="n">
-        <v>50</v>
+        <v>50.11538314819336</v>
       </c>
       <c r="D27" t="n">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -846,13 +846,13 @@
         <v>11.5</v>
       </c>
       <c r="C28" t="n">
-        <v>50</v>
+        <v>50.11538314819336</v>
       </c>
       <c r="D28" t="n">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -863,13 +863,13 @@
         <v>12</v>
       </c>
       <c r="C29" t="n">
-        <v>50</v>
+        <v>50.11538314819336</v>
       </c>
       <c r="D29" t="n">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -880,13 +880,13 @@
         <v>12.5</v>
       </c>
       <c r="C30" t="n">
-        <v>49.96126937866211</v>
+        <v>50.11538314819336</v>
       </c>
       <c r="D30" t="n">
         <v>2030</v>
       </c>
       <c r="E30" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -897,13 +897,13 @@
         <v>13</v>
       </c>
       <c r="C31" t="n">
-        <v>49.96126937866211</v>
+        <v>50.07692337036133</v>
       </c>
       <c r="D31" t="n">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="E31" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -914,13 +914,13 @@
         <v>13.5</v>
       </c>
       <c r="C32" t="n">
-        <v>49.96126937866211</v>
+        <v>50.11538314819336</v>
       </c>
       <c r="D32" t="n">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="E32" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -931,13 +931,13 @@
         <v>14</v>
       </c>
       <c r="C33" t="n">
-        <v>49.92254257202148</v>
+        <v>50.07692337036133</v>
       </c>
       <c r="D33" t="n">
         <v>2029</v>
       </c>
       <c r="E33" t="n">
-        <v>-2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -948,13 +948,13 @@
         <v>14.5</v>
       </c>
       <c r="C34" t="n">
-        <v>49.92254257202148</v>
+        <v>50.03845977783203</v>
       </c>
       <c r="D34" t="n">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="E34" t="n">
-        <v>-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -965,13 +965,13 @@
         <v>15</v>
       </c>
       <c r="C35" t="n">
-        <v>49.92254257202148</v>
+        <v>50.03845977783203</v>
       </c>
       <c r="D35" t="n">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="E35" t="n">
-        <v>-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -982,13 +982,13 @@
         <v>15.5</v>
       </c>
       <c r="C36" t="n">
-        <v>49.88381195068359</v>
+        <v>50.03845977783203</v>
       </c>
       <c r="D36" t="n">
         <v>2028</v>
       </c>
       <c r="E36" t="n">
-        <v>-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -999,13 +999,13 @@
         <v>16</v>
       </c>
       <c r="C37" t="n">
-        <v>49.88381195068359</v>
+        <v>50</v>
       </c>
       <c r="D37" t="n">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="E37" t="n">
-        <v>-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1036,16 +1036,16 @@
         <v>8</v>
       </c>
       <c r="C40" t="n">
-        <v>100.0386047363281</v>
+        <v>100</v>
       </c>
       <c r="D40" t="n">
         <v>3327</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>3326</v>
+        <v>3327</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1056,13 +1056,13 @@
         <v>8.5</v>
       </c>
       <c r="C41" t="n">
-        <v>100.0386047363281</v>
+        <v>100</v>
       </c>
       <c r="D41" t="n">
         <v>3327</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1073,13 +1073,13 @@
         <v>9</v>
       </c>
       <c r="C42" t="n">
-        <v>100.0386047363281</v>
+        <v>100</v>
       </c>
       <c r="D42" t="n">
         <v>3327</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1090,13 +1090,13 @@
         <v>9.5</v>
       </c>
       <c r="C43" t="n">
-        <v>100.0386047363281</v>
+        <v>100</v>
       </c>
       <c r="D43" t="n">
         <v>3327</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1107,13 +1107,13 @@
         <v>10</v>
       </c>
       <c r="C44" t="n">
-        <v>100.0386047363281</v>
+        <v>100</v>
       </c>
       <c r="D44" t="n">
         <v>3327</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1124,13 +1124,13 @@
         <v>10.5</v>
       </c>
       <c r="C45" t="n">
-        <v>100.0386047363281</v>
+        <v>100</v>
       </c>
       <c r="D45" t="n">
         <v>3327</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1141,13 +1141,13 @@
         <v>11</v>
       </c>
       <c r="C46" t="n">
-        <v>100.0386047363281</v>
+        <v>99.96154022216797</v>
       </c>
       <c r="D46" t="n">
-        <v>3327</v>
+        <v>3326</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1158,13 +1158,13 @@
         <v>11.5</v>
       </c>
       <c r="C47" t="n">
-        <v>100</v>
+        <v>99.96154022216797</v>
       </c>
       <c r="D47" t="n">
         <v>3326</v>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1175,13 +1175,13 @@
         <v>12</v>
       </c>
       <c r="C48" t="n">
-        <v>100</v>
+        <v>99.92308044433594</v>
       </c>
       <c r="D48" t="n">
-        <v>3326</v>
+        <v>3325</v>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1192,13 +1192,13 @@
         <v>12.5</v>
       </c>
       <c r="C49" t="n">
-        <v>99.96139526367188</v>
+        <v>99.92308044433594</v>
       </c>
       <c r="D49" t="n">
         <v>3325</v>
       </c>
       <c r="E49" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1209,13 +1209,13 @@
         <v>13</v>
       </c>
       <c r="C50" t="n">
-        <v>99.96139526367188</v>
+        <v>99.88461303710938</v>
       </c>
       <c r="D50" t="n">
-        <v>3325</v>
+        <v>3324</v>
       </c>
       <c r="E50" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1226,13 +1226,13 @@
         <v>13.5</v>
       </c>
       <c r="C51" t="n">
-        <v>99.92277526855469</v>
+        <v>99.88461303710938</v>
       </c>
       <c r="D51" t="n">
         <v>3324</v>
       </c>
       <c r="E51" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1243,13 +1243,13 @@
         <v>14</v>
       </c>
       <c r="C52" t="n">
-        <v>99.88417053222656</v>
+        <v>99.84615325927734</v>
       </c>
       <c r="D52" t="n">
         <v>3323</v>
       </c>
       <c r="E52" t="n">
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1260,13 +1260,13 @@
         <v>14.5</v>
       </c>
       <c r="C53" t="n">
-        <v>99.88417053222656</v>
+        <v>99.80769348144531</v>
       </c>
       <c r="D53" t="n">
-        <v>3323</v>
+        <v>3322</v>
       </c>
       <c r="E53" t="n">
-        <v>-3</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1277,13 +1277,13 @@
         <v>15</v>
       </c>
       <c r="C54" t="n">
-        <v>99.84555816650391</v>
+        <v>99.80769348144531</v>
       </c>
       <c r="D54" t="n">
         <v>3322</v>
       </c>
       <c r="E54" t="n">
-        <v>-4</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1294,13 +1294,13 @@
         <v>15.5</v>
       </c>
       <c r="C55" t="n">
-        <v>99.80694580078125</v>
+        <v>99.76922607421875</v>
       </c>
       <c r="D55" t="n">
-        <v>3322</v>
+        <v>3321</v>
       </c>
       <c r="E55" t="n">
-        <v>-4</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1311,13 +1311,13 @@
         <v>16</v>
       </c>
       <c r="C56" t="n">
-        <v>99.76834106445312</v>
+        <v>99.73077392578125</v>
       </c>
       <c r="D56" t="n">
         <v>3320</v>
       </c>
       <c r="E56" t="n">
-        <v>-6</v>
+        <v>-7</v>
       </c>
     </row>
   </sheetData>
@@ -1387,13 +1387,13 @@
         <v>16.5</v>
       </c>
       <c r="C3" t="n">
-        <v>0.03891050443053246</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1404,13 +1404,13 @@
         <v>17</v>
       </c>
       <c r="C4" t="n">
-        <v>0.03891050443053246</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1421,13 +1421,13 @@
         <v>17.5</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>-0.03891050443053246</v>
       </c>
       <c r="D5" t="n">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1438,13 +1438,13 @@
         <v>18</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>-0.03891050443053246</v>
       </c>
       <c r="D6" t="n">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1455,13 +1455,13 @@
         <v>18.5</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>-0.03891050443053246</v>
       </c>
       <c r="D7" t="n">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1472,13 +1472,13 @@
         <v>19</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>-0.07782100886106491</v>
       </c>
       <c r="D8" t="n">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1489,13 +1489,13 @@
         <v>19.5</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.03891050443053246</v>
+        <v>-0.07782100886106491</v>
       </c>
       <c r="D9" t="n">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E9" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1506,13 +1506,13 @@
         <v>20</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.03891050443053246</v>
+        <v>-0.07782100886106491</v>
       </c>
       <c r="D10" t="n">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E10" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1523,13 +1523,13 @@
         <v>20.5</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.03891050443053246</v>
+        <v>-0.07782100886106491</v>
       </c>
       <c r="D11" t="n">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E11" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1540,13 +1540,13 @@
         <v>21</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.03891050443053246</v>
+        <v>-0.1167315170168877</v>
       </c>
       <c r="D12" t="n">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E12" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1557,13 +1557,13 @@
         <v>21.5</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.03891050443053246</v>
+        <v>-0.1167315170168877</v>
       </c>
       <c r="D13" t="n">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E13" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1574,13 +1574,13 @@
         <v>22</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.03891050443053246</v>
+        <v>-0.1167315170168877</v>
       </c>
       <c r="D14" t="n">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E14" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1591,13 +1591,13 @@
         <v>22.5</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.07782100886106491</v>
+        <v>-0.1167315170168877</v>
       </c>
       <c r="D15" t="n">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E15" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1608,13 +1608,13 @@
         <v>23</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.07782100886106491</v>
+        <v>-0.1556420177221298</v>
       </c>
       <c r="D16" t="n">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="E16" t="n">
-        <v>-2</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1625,13 +1625,13 @@
         <v>23.5</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.07782100886106491</v>
+        <v>-0.1556420177221298</v>
       </c>
       <c r="D17" t="n">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E17" t="n">
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1642,13 +1642,13 @@
         <v>24</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.1167315170168877</v>
+        <v>-0.1556420177221298</v>
       </c>
       <c r="D18" t="n">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E18" t="n">
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1679,7 +1679,7 @@
         <v>16</v>
       </c>
       <c r="C21" t="n">
-        <v>50.19379806518555</v>
+        <v>50.15515899658203</v>
       </c>
       <c r="D21" t="n">
         <v>2027</v>
@@ -1699,13 +1699,13 @@
         <v>16.5</v>
       </c>
       <c r="C22" t="n">
-        <v>50.15503692626953</v>
+        <v>50.15515899658203</v>
       </c>
       <c r="D22" t="n">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1716,7 +1716,7 @@
         <v>17</v>
       </c>
       <c r="C23" t="n">
-        <v>50.11627960205078</v>
+        <v>50.11637115478516</v>
       </c>
       <c r="D23" t="n">
         <v>2026</v>
@@ -1733,13 +1733,13 @@
         <v>17.5</v>
       </c>
       <c r="C24" t="n">
-        <v>50.11627960205078</v>
+        <v>50.07757949829102</v>
       </c>
       <c r="D24" t="n">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1750,7 +1750,7 @@
         <v>18</v>
       </c>
       <c r="C25" t="n">
-        <v>50.07751846313477</v>
+        <v>50.07757949829102</v>
       </c>
       <c r="D25" t="n">
         <v>2025</v>
@@ -1767,7 +1767,7 @@
         <v>18.5</v>
       </c>
       <c r="C26" t="n">
-        <v>50.03876113891602</v>
+        <v>50.03879165649414</v>
       </c>
       <c r="D26" t="n">
         <v>2024</v>
@@ -1784,7 +1784,7 @@
         <v>19</v>
       </c>
       <c r="C27" t="n">
-        <v>50.03876113891602</v>
+        <v>50.03879165649414</v>
       </c>
       <c r="D27" t="n">
         <v>2024</v>
@@ -1852,13 +1852,13 @@
         <v>21</v>
       </c>
       <c r="C31" t="n">
-        <v>49.96109008789062</v>
+        <v>49.92218017578125</v>
       </c>
       <c r="D31" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="E31" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1991,16 +1991,16 @@
         <v>16</v>
       </c>
       <c r="C40" t="n">
-        <v>100.2713165283203</v>
+        <v>100.3103179931641</v>
       </c>
       <c r="D40" t="n">
         <v>3320</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F40" t="n">
-        <v>3313</v>
+        <v>3312</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2011,13 +2011,13 @@
         <v>16.5</v>
       </c>
       <c r="C41" t="n">
-        <v>100.2325592041016</v>
+        <v>100.2715301513672</v>
       </c>
       <c r="D41" t="n">
         <v>3319</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2028,13 +2028,13 @@
         <v>17</v>
       </c>
       <c r="C42" t="n">
-        <v>100.1938018798828</v>
+        <v>100.2327423095703</v>
       </c>
       <c r="D42" t="n">
         <v>3318</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2045,13 +2045,13 @@
         <v>17.5</v>
       </c>
       <c r="C43" t="n">
-        <v>100.1550369262695</v>
+        <v>100.155158996582</v>
       </c>
       <c r="D43" t="n">
         <v>3317</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2062,13 +2062,13 @@
         <v>18</v>
       </c>
       <c r="C44" t="n">
-        <v>100.1162796020508</v>
+        <v>100.155158996582</v>
       </c>
       <c r="D44" t="n">
         <v>3316</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2079,13 +2079,13 @@
         <v>18.5</v>
       </c>
       <c r="C45" t="n">
-        <v>100.0775146484375</v>
+        <v>100.1163711547852</v>
       </c>
       <c r="D45" t="n">
         <v>3315</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2096,10 +2096,10 @@
         <v>19</v>
       </c>
       <c r="C46" t="n">
-        <v>100.0775146484375</v>
+        <v>100.0775756835938</v>
       </c>
       <c r="D46" t="n">
-        <v>3315</v>
+        <v>3314</v>
       </c>
       <c r="E46" t="n">
         <v>2</v>
@@ -2113,10 +2113,10 @@
         <v>19.5</v>
       </c>
       <c r="C47" t="n">
-        <v>100.0387573242188</v>
+        <v>100.0387878417969</v>
       </c>
       <c r="D47" t="n">
-        <v>3314</v>
+        <v>3313</v>
       </c>
       <c r="E47" t="n">
         <v>1</v>
@@ -2133,7 +2133,7 @@
         <v>100</v>
       </c>
       <c r="D48" t="n">
-        <v>3313</v>
+        <v>3312</v>
       </c>
       <c r="E48" t="n">
         <v>0</v>
@@ -2147,10 +2147,10 @@
         <v>20.5</v>
       </c>
       <c r="C49" t="n">
-        <v>99.96124267578125</v>
+        <v>99.96121215820312</v>
       </c>
       <c r="D49" t="n">
-        <v>3312</v>
+        <v>3311</v>
       </c>
       <c r="E49" t="n">
         <v>-1</v>
@@ -2164,13 +2164,13 @@
         <v>21</v>
       </c>
       <c r="C50" t="n">
-        <v>99.88372039794922</v>
+        <v>99.92242431640625</v>
       </c>
       <c r="D50" t="n">
         <v>3310</v>
       </c>
       <c r="E50" t="n">
-        <v>-3</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2181,10 +2181,10 @@
         <v>21.5</v>
       </c>
       <c r="C51" t="n">
-        <v>99.88372039794922</v>
+        <v>99.88362884521484</v>
       </c>
       <c r="D51" t="n">
-        <v>3310</v>
+        <v>3309</v>
       </c>
       <c r="E51" t="n">
         <v>-3</v>
@@ -2198,10 +2198,10 @@
         <v>22</v>
       </c>
       <c r="C52" t="n">
-        <v>99.84496307373047</v>
+        <v>99.84484100341797</v>
       </c>
       <c r="D52" t="n">
-        <v>3309</v>
+        <v>3308</v>
       </c>
       <c r="E52" t="n">
         <v>-4</v>
@@ -2215,10 +2215,10 @@
         <v>22.5</v>
       </c>
       <c r="C53" t="n">
-        <v>99.76744079589844</v>
+        <v>99.84484100341797</v>
       </c>
       <c r="D53" t="n">
-        <v>3308</v>
+        <v>3307</v>
       </c>
       <c r="E53" t="n">
         <v>-5</v>
@@ -2232,10 +2232,10 @@
         <v>23</v>
       </c>
       <c r="C54" t="n">
-        <v>99.76744079589844</v>
+        <v>99.76725769042969</v>
       </c>
       <c r="D54" t="n">
-        <v>3307</v>
+        <v>3306</v>
       </c>
       <c r="E54" t="n">
         <v>-6</v>
@@ -2249,13 +2249,13 @@
         <v>23.5</v>
       </c>
       <c r="C55" t="n">
-        <v>99.72868347167969</v>
+        <v>99.76725769042969</v>
       </c>
       <c r="D55" t="n">
         <v>3306</v>
       </c>
       <c r="E55" t="n">
-        <v>-7</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2266,13 +2266,13 @@
         <v>24</v>
       </c>
       <c r="C56" t="n">
-        <v>99.68992614746094</v>
+        <v>99.72846984863281</v>
       </c>
       <c r="D56" t="n">
         <v>3305</v>
       </c>
       <c r="E56" t="n">
-        <v>-8</v>
+        <v>-7</v>
       </c>
     </row>
   </sheetData>
@@ -2322,16 +2322,16 @@
         <v>22</v>
       </c>
       <c r="C2" t="n">
-        <v>0.07806400954723358</v>
+        <v>0.0390625</v>
       </c>
       <c r="D2" t="n">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>735</v>
+        <v>736</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2342,13 +2342,13 @@
         <v>22.5</v>
       </c>
       <c r="C3" t="n">
-        <v>0.03903200477361679</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>736</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2359,13 +2359,13 @@
         <v>23</v>
       </c>
       <c r="C4" t="n">
-        <v>0.03903200477361679</v>
+        <v>-0.0390625</v>
       </c>
       <c r="D4" t="n">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2376,13 +2376,13 @@
         <v>23.5</v>
       </c>
       <c r="C5" t="n">
-        <v>0.03903200477361679</v>
+        <v>-0.0390625</v>
       </c>
       <c r="D5" t="n">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2393,13 +2393,13 @@
         <v>24</v>
       </c>
       <c r="C6" t="n">
-        <v>0.03903200477361679</v>
+        <v>-0.0390625</v>
       </c>
       <c r="D6" t="n">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2410,13 +2410,13 @@
         <v>24.5</v>
       </c>
       <c r="C7" t="n">
-        <v>0.03903200477361679</v>
+        <v>-0.078125</v>
       </c>
       <c r="D7" t="n">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2427,13 +2427,13 @@
         <v>25</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>-0.078125</v>
       </c>
       <c r="D8" t="n">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2444,13 +2444,13 @@
         <v>25.5</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>-0.078125</v>
       </c>
       <c r="D9" t="n">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2461,13 +2461,13 @@
         <v>26</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>-0.1171875</v>
       </c>
       <c r="D10" t="n">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2478,13 +2478,13 @@
         <v>26.5</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.03903200477361679</v>
+        <v>-0.1171875</v>
       </c>
       <c r="D11" t="n">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E11" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2495,13 +2495,13 @@
         <v>27</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.03903200477361679</v>
+        <v>-0.1171875</v>
       </c>
       <c r="D12" t="n">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E12" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2512,13 +2512,13 @@
         <v>27.5</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.03903200477361679</v>
+        <v>-0.1171875</v>
       </c>
       <c r="D13" t="n">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E13" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2529,13 +2529,13 @@
         <v>28</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.03903200477361679</v>
+        <v>-0.15625</v>
       </c>
       <c r="D14" t="n">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="E14" t="n">
-        <v>-1</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2546,13 +2546,13 @@
         <v>28.5</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.07806400954723358</v>
+        <v>-0.15625</v>
       </c>
       <c r="D15" t="n">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E15" t="n">
-        <v>-2</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2563,13 +2563,13 @@
         <v>29</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.07806400954723358</v>
+        <v>-0.15625</v>
       </c>
       <c r="D16" t="n">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E16" t="n">
-        <v>-2</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2580,13 +2580,13 @@
         <v>29.5</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.07806400954723358</v>
+        <v>-0.15625</v>
       </c>
       <c r="D17" t="n">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E17" t="n">
-        <v>-2</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2597,13 +2597,13 @@
         <v>30</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.07806400954723358</v>
+        <v>-0.15625</v>
       </c>
       <c r="D18" t="n">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E18" t="n">
-        <v>-2</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2654,13 +2654,13 @@
         <v>22.5</v>
       </c>
       <c r="C22" t="n">
-        <v>50.15564346313477</v>
+        <v>50.11672973632812</v>
       </c>
       <c r="D22" t="n">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2722,13 +2722,13 @@
         <v>24.5</v>
       </c>
       <c r="C26" t="n">
-        <v>50.07781982421875</v>
+        <v>50.03890991210938</v>
       </c>
       <c r="D26" t="n">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2773,13 +2773,13 @@
         <v>26</v>
       </c>
       <c r="C29" t="n">
-        <v>50</v>
+        <v>49.9609375</v>
       </c>
       <c r="D29" t="n">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2790,7 +2790,7 @@
         <v>26.5</v>
       </c>
       <c r="C30" t="n">
-        <v>49.96096801757812</v>
+        <v>49.9609375</v>
       </c>
       <c r="D30" t="n">
         <v>2015</v>
@@ -2807,7 +2807,7 @@
         <v>27</v>
       </c>
       <c r="C31" t="n">
-        <v>49.92193603515625</v>
+        <v>49.921875</v>
       </c>
       <c r="D31" t="n">
         <v>2014</v>
@@ -2824,13 +2824,13 @@
         <v>27.5</v>
       </c>
       <c r="C32" t="n">
-        <v>49.92193603515625</v>
+        <v>49.8828125</v>
       </c>
       <c r="D32" t="n">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="E32" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2841,7 +2841,7 @@
         <v>28</v>
       </c>
       <c r="C33" t="n">
-        <v>49.88290405273438</v>
+        <v>49.8828125</v>
       </c>
       <c r="D33" t="n">
         <v>2013</v>
@@ -2858,7 +2858,7 @@
         <v>28.5</v>
       </c>
       <c r="C34" t="n">
-        <v>49.88290405273438</v>
+        <v>49.8828125</v>
       </c>
       <c r="D34" t="n">
         <v>2013</v>
@@ -2875,7 +2875,7 @@
         <v>29</v>
       </c>
       <c r="C35" t="n">
-        <v>49.8438720703125</v>
+        <v>49.84375</v>
       </c>
       <c r="D35" t="n">
         <v>2012</v>
@@ -2892,7 +2892,7 @@
         <v>29.5</v>
       </c>
       <c r="C36" t="n">
-        <v>49.80484008789062</v>
+        <v>49.8046875</v>
       </c>
       <c r="D36" t="n">
         <v>2011</v>
@@ -2909,7 +2909,7 @@
         <v>30</v>
       </c>
       <c r="C37" t="n">
-        <v>49.80484008789062</v>
+        <v>49.8046875</v>
       </c>
       <c r="D37" t="n">
         <v>2011</v>
@@ -2946,13 +2946,13 @@
         <v>22</v>
       </c>
       <c r="C40" t="n">
-        <v>100.311279296875</v>
+        <v>100.2723693847656</v>
       </c>
       <c r="D40" t="n">
-        <v>3309</v>
+        <v>3308</v>
       </c>
       <c r="E40" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
         <v>3301</v>
@@ -2986,10 +2986,10 @@
         <v>100.1945495605469</v>
       </c>
       <c r="D42" t="n">
-        <v>3307</v>
+        <v>3306</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -3017,13 +3017,13 @@
         <v>24</v>
       </c>
       <c r="C44" t="n">
-        <v>100.1556396484375</v>
+        <v>100.1167297363281</v>
       </c>
       <c r="D44" t="n">
-        <v>3305</v>
+        <v>3304</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -3034,13 +3034,13 @@
         <v>24.5</v>
       </c>
       <c r="C45" t="n">
-        <v>100.1167297363281</v>
+        <v>100.0778198242188</v>
       </c>
       <c r="D45" t="n">
-        <v>3304</v>
+        <v>3303</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -3051,13 +3051,13 @@
         <v>25</v>
       </c>
       <c r="C46" t="n">
-        <v>100.0778198242188</v>
+        <v>100.0389099121094</v>
       </c>
       <c r="D46" t="n">
-        <v>3303</v>
+        <v>3302</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -3085,13 +3085,13 @@
         <v>26</v>
       </c>
       <c r="C48" t="n">
-        <v>100</v>
+        <v>99.96109008789062</v>
       </c>
       <c r="D48" t="n">
-        <v>3301</v>
+        <v>3300</v>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -3102,13 +3102,13 @@
         <v>26.5</v>
       </c>
       <c r="C49" t="n">
-        <v>99.96109008789062</v>
+        <v>99.92218017578125</v>
       </c>
       <c r="D49" t="n">
-        <v>3300</v>
+        <v>3299</v>
       </c>
       <c r="E49" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -3119,13 +3119,13 @@
         <v>27</v>
       </c>
       <c r="C50" t="n">
-        <v>99.92218017578125</v>
+        <v>99.88327026367188</v>
       </c>
       <c r="D50" t="n">
-        <v>3299</v>
+        <v>3298</v>
       </c>
       <c r="E50" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -3136,13 +3136,13 @@
         <v>27.5</v>
       </c>
       <c r="C51" t="n">
-        <v>99.88327026367188</v>
+        <v>99.8443603515625</v>
       </c>
       <c r="D51" t="n">
-        <v>3298</v>
+        <v>3297</v>
       </c>
       <c r="E51" t="n">
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -3153,7 +3153,7 @@
         <v>28</v>
       </c>
       <c r="C52" t="n">
-        <v>99.80545043945312</v>
+        <v>99.8443603515625</v>
       </c>
       <c r="D52" t="n">
         <v>3297</v>
@@ -3187,13 +3187,13 @@
         <v>29</v>
       </c>
       <c r="C54" t="n">
-        <v>99.76654052734375</v>
+        <v>99.72763061523438</v>
       </c>
       <c r="D54" t="n">
-        <v>3295</v>
+        <v>3294</v>
       </c>
       <c r="E54" t="n">
-        <v>-6</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -3204,13 +3204,13 @@
         <v>29.5</v>
       </c>
       <c r="C55" t="n">
-        <v>99.72763061523438</v>
+        <v>99.688720703125</v>
       </c>
       <c r="D55" t="n">
-        <v>3294</v>
+        <v>3293</v>
       </c>
       <c r="E55" t="n">
-        <v>-7</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -3221,13 +3221,13 @@
         <v>30</v>
       </c>
       <c r="C56" t="n">
-        <v>99.688720703125</v>
+        <v>99.64981079101562</v>
       </c>
       <c r="D56" t="n">
-        <v>3293</v>
+        <v>3292</v>
       </c>
       <c r="E56" t="n">
-        <v>-8</v>
+        <v>-9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>